<commit_message>
everything put into functions scribble
</commit_message>
<xml_diff>
--- a/ColumnLogbook_QR.xlsx
+++ b/ColumnLogbook_QR.xlsx
@@ -412,13 +412,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.75"/>
+  <cols>
+    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.31640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.90625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="4.54296875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.76953125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8.76953125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="16" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="34.40625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="35.76953125" bestFit="1" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -509,147 +520,6 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>Great it was a pleasure working with you</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Patricia Brown </t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2024-06-28 </t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEC-17 </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">6 </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.5 </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">no </t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ethanol solution </t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Great it was a pleasure working with you</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Patricia Brown </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2024-06-28 </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEC-17 </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">6 </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.5 </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">no </t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ethanol solution </t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Great it was a pleasure working with you</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Patricia Brown </t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2024-06-28 </t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEC-17 </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">6 </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.5 </t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">no </t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ethanol solution </t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>Great it was a pleasure working with you</t>
         </is>

</xml_diff>

<commit_message>
improved version works now
</commit_message>
<xml_diff>
--- a/ColumnLogbook_QR.xlsx
+++ b/ColumnLogbook_QR.xlsx
@@ -412,23 +412,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="10.31640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="11.90625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="4.54296875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="11.76953125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="8.76953125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="16" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="34.40625" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="35.76953125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="19.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="12.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="4.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="12.42578125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="10.5703125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="16.85546875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="36.140625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="86.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,59 +469,556 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>solution equilibratedErrors/Comments</t>
+          <t>solution equilibrated</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>comments</t>
+          <t>Errors/Comments</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Patricia Brown </t>
+          <t xml:space="preserve">Patricia 
+</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">2024-06-28 </t>
+          <t xml:space="preserve">2024-06-28 
+</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEC-17 </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">6 </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.5 </t>
+          <t xml:space="preserve">SEC-17 
+</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">no </t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ethanol solution </t>
+          <t xml:space="preserve">1 
+</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Great it was a pleasure working with you</t>
+          <t>Great</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Testing 
+</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-07-02 
+</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-01 
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 
+</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>all good</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pat  
+</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-07-02 
+</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-11 
+</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 
+</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>All good</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patricia  
+</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-07-24 
+</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-06 
+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5 
+</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.3 
+</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.2 
+</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">yes 
+</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethanol 
+</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>High pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emanuel Bruckisch 
+</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-07-30 
+</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-06 
+</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no 
+</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">True buffer 
+</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Left on buffer for Lukas to use next</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nele 
+</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-07 
+</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-12 
+</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4 
+</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1.96 
+</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.2 
+</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Konrad  
+</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-15 
+</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-14 
+</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 
+</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.72 
+</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.2 
+</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">yes 
+</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethanol  
+</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Flowrate on chart (0.4 ml/min) resulted in overpresser. Had to reduce to 0.2 for good pressure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Konrad  
+</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-15 
+</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-13 
+</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 
+</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.72 
+</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.2 
+</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">yes 
+</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethanol  
+</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Flowrate on chart (0.4 ml/min) resulted in overpresser. Had to reduce to 0.2 for good pressure.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Konrad  
+</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-13 
+</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AX-02 
+</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 
+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3.6 
+</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2.5 
+</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">yes 
+</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Water  
+</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Cleaned with 2M NaCl</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lukas 
+</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-22 
+</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-06 
+</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 
+</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.12 - 0.19 
+</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.5 - 0.7 
+</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>All good</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emanuel Bruckisch 
+</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-28 
+</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-04 
+</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emanuel Bruckisch 
+</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-28 
+</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEC-04 
+</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emanuel Bruckisch 
+</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024-08-29 
+</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CX-01 
+</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 
+</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.17 Mpa 
+</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 ml/min 
+</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no 
+</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Etoh 
+</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Not yet regenerated with high NaCl buffer</t>
         </is>
       </c>
     </row>

</xml_diff>